<commit_message>
solve simplex rhs bugs
</commit_message>
<xml_diff>
--- a/readfile.xlsx
+++ b/readfile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\semester 5\operation Research\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F95B94DB-D233-41DB-9CBB-8388B31E47DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C732D3DF-E131-4FA4-B9B8-BF806AC1CBE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17160" yWindow="2000" windowWidth="7370" windowHeight="11170" xr2:uid="{3D034782-3DDE-4971-9DBF-CAA6E7819B91}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t>result</t>
   </si>
@@ -436,10 +436,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1"/>
       <c r="E2" s="2"/>
@@ -449,10 +449,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C3" s="1">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>3</v>
@@ -460,31 +460,23 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B4" s="1">
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="C4" s="1">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="1">
-        <v>1</v>
-      </c>
-      <c r="B5" s="1">
-        <v>1</v>
-      </c>
-      <c r="C5" s="1">
-        <v>9</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="E5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
simplex run on diff examples
</commit_message>
<xml_diff>
--- a/readfile.xlsx
+++ b/readfile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\semester 5\operation Research\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B12C021-F002-4AE5-89BE-5771164D52E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E501857D-15EA-4615-89FF-7AF7872D6C5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17160" yWindow="2000" windowWidth="7370" windowHeight="11170" xr2:uid="{3D034782-3DDE-4971-9DBF-CAA6E7819B91}"/>
   </bookViews>
@@ -436,23 +436,23 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="1"/>
       <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
+        <v>-1</v>
+      </c>
+      <c r="B3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="1">
-        <v>4</v>
-      </c>
       <c r="C3" s="1">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>3</v>
@@ -460,13 +460,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
       </c>
       <c r="C4" s="1">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>3</v>
@@ -474,13 +474,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C5" s="1">
-        <v>9</v>
+        <v>90</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>3</v>

</xml_diff>